<commit_message>
thêm dữ liệu mẫu cho file excel và fix đường dẫn bình luận
</commit_message>
<xml_diff>
--- a/HeThongQuanLyBaiGiang/public/BaiKiemTra/Template_Import_BaiKiemTra.xlsx
+++ b/HeThongQuanLyBaiGiang/public/BaiKiemTra/Template_Import_BaiKiemTra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATN\HeThongQuanLyBaiGiang\HeThongQuanLyBaiGiang\public\BaiKiemTra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ABC9C1-FCA4-453F-A0E4-E41B1BCD21D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3C0CCA-A970-4FF7-8016-6D41DF2B8F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB34626C-C1EA-40C1-A7C5-C8434FF17F28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Tên bài kiểm tra</t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t>Đáp án đúng</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy HH:mm:ss</t>
+  </si>
+  <si>
+    <t>Mô tả bài kiểm tra</t>
+  </si>
+  <si>
+    <t>Hiện / Ẩn</t>
+  </si>
+  <si>
+    <t>(Đây là dữ liệu mẫu, vui lòng hãy xóa để thêm mới)</t>
   </si>
 </sst>
 </file>
@@ -76,7 +88,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +108,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -228,12 +248,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -248,6 +262,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,7 +586,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -575,82 +595,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>14</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2"/>
     </row>
     <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3"/>
     </row>
     <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
update import, export bài kiểm tra
</commit_message>
<xml_diff>
--- a/HeThongQuanLyBaiGiang/public/BaiKiemTra/Template_Import_BaiKiemTra.xlsx
+++ b/HeThongQuanLyBaiGiang/public/BaiKiemTra/Template_Import_BaiKiemTra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATN\HeThongQuanLyBaiGiang\HeThongQuanLyBaiGiang\public\BaiKiemTra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3C0CCA-A970-4FF7-8016-6D41DF2B8F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2429130-68EB-4F47-921F-2320ED337733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB34626C-C1EA-40C1-A7C5-C8434FF17F28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Tên bài kiểm tra</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>(Đây là dữ liệu mẫu, vui lòng hãy xóa để thêm mới)</t>
+  </si>
+  <si>
+    <t>Cho phép xem kết quả</t>
+  </si>
+  <si>
+    <t>Thời gian làm bài (phút)</t>
+  </si>
+  <si>
+    <t>Từ 15 - 180</t>
+  </si>
+  <si>
+    <t>Có / Không</t>
   </si>
 </sst>
 </file>
@@ -245,12 +257,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -263,11 +269,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1011ED2E-E1A2-4863-B6FB-F1273005A9AF}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -595,21 +607,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1"/>
     </row>
     <row r="2" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="10"/>
@@ -621,7 +633,7 @@
       <c r="F2"/>
     </row>
     <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="10"/>
@@ -633,10 +645,10 @@
       <c r="F3"/>
     </row>
     <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
@@ -645,54 +657,85 @@
       <c r="F4"/>
     </row>
     <row r="5" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5"/>
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="11"/>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6"/>
+    </row>
+    <row r="7" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F8" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Đáp án không hợp lệ&quot;" error="&quot;Đáp án chỉ chấp nhận A, B, C, D&quot;" sqref="F7:F1048576" xr:uid="{5A7367E5-F854-4F07-848F-DB0768AAE1CB}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Đáp án không hợp lệ&quot;" error="&quot;Đáp án chỉ chấp nhận A, B, C, D&quot;" sqref="F9:F1048576" xr:uid="{5A7367E5-F854-4F07-848F-DB0768AAE1CB}">
       <formula1>"a,b,c,d,A,B,C,D"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Trạng thái không hợp lệ&quot;" error="&quot;Trạng thái chỉ chấp nhận Ẩn hoặc Hiện&quot;" sqref="B5" xr:uid="{AFAC3057-0DE7-4235-B898-5DEF661569B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Trạng thái không hợp lệ&quot;" error="&quot;Trạng thái chỉ chấp nhận Ẩn hoặc Hiện&quot;" sqref="B7" xr:uid="{AFAC3057-0DE7-4235-B898-5DEF661569B3}">
       <formula1>"Ẩn,Hiện"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Cho phép xem kết quả: lỗi&quot;" error="&quot;Cho phép xem kết quả không hợp lệ, chỉ chấp nhận giá trị Có hoặc Không&quot;" sqref="B6" xr:uid="{110F3508-9495-45D6-AFA0-DFC7A98731C3}">
+      <formula1>"Có,Không"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Thời gian làm bài không hợp lệ&quot;" error="&quot;Thời gian chỉ chấp nhận từ 15 đến 180 phút&quot;" sqref="B5" xr:uid="{02A06E6E-67B6-49DC-AE25-1E55121676CC}">
+      <formula1>15</formula1>
+      <formula2>180</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update bài kiểm tra
</commit_message>
<xml_diff>
--- a/HeThongQuanLyBaiGiang/public/BaiKiemTra/Template_Import_BaiKiemTra.xlsx
+++ b/HeThongQuanLyBaiGiang/public/BaiKiemTra/Template_Import_BaiKiemTra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATN\HeThongQuanLyBaiGiang\HeThongQuanLyBaiGiang\public\BaiKiemTra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2429130-68EB-4F47-921F-2320ED337733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CDD6A2-7E7E-4902-969A-2848D1EE17AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB34626C-C1EA-40C1-A7C5-C8434FF17F28}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>Hiện / Ẩn</t>
   </si>
   <si>
-    <t>(Đây là dữ liệu mẫu, vui lòng hãy xóa để thêm mới)</t>
-  </si>
-  <si>
     <t>Cho phép xem kết quả</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Có / Không</t>
+  </si>
+  <si>
+    <t>(Đây là dữ liệu mẫu, vui lòng hãy xóa để thêm mới. Nếu chỉ import câu hỏi bài kiểm tra thì có thể bỏ trống thông tin bài kiểm tra)</t>
   </si>
 </sst>
 </file>
@@ -154,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -242,11 +242,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -269,9 +278,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -280,6 +286,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,7 +612,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -610,12 +624,12 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>14</v>
+      <c r="D1" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1"/>
@@ -624,11 +638,11 @@
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="2"/>
       <c r="F2"/>
     </row>
@@ -636,11 +650,11 @@
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="2"/>
       <c r="F3"/>
     </row>
@@ -648,35 +662,35 @@
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="1"/>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="1"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="B6" s="10"/>
       <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="D6" s="11"/>
       <c r="E6" s="1"/>
       <c r="F6"/>
     </row>
@@ -684,11 +698,11 @@
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="1"/>
       <c r="F7"/>
     </row>
@@ -722,6 +736,9 @@
     </row>
   </sheetData>
   <dataConsolidate/>
+  <mergeCells count="1">
+    <mergeCell ref="D1:D7"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="&quot;Đáp án không hợp lệ&quot;" error="&quot;Đáp án chỉ chấp nhận A, B, C, D&quot;" sqref="F9:F1048576" xr:uid="{5A7367E5-F854-4F07-848F-DB0768AAE1CB}">

</xml_diff>